<commit_message>
Sprint 2 - Se crean los test de CP y NIF
</commit_message>
<xml_diff>
--- a/docs/CasosPrueba - Validación/CP - Código Postal.xlsx
+++ b/docs/CasosPrueba - Validación/CP - Código Postal.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adri_\source\repos\TDD-ACB-JGA\docs\CasosPrueba - Validación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D1B9E4-1CD1-432E-8E93-64B1769D6156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AE4D66-7754-4926-999D-8000A6D75B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
+    <workbookView xWindow="14835" yWindow="330" windowWidth="13785" windowHeight="15030" activeTab="2" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
   </bookViews>
   <sheets>
     <sheet name="CP-VAL-CP-001" sheetId="1" r:id="rId1"/>
     <sheet name="CP-VAL-CP-002" sheetId="11" r:id="rId2"/>
-    <sheet name="CP-VAL-CP-003" sheetId="13" r:id="rId3"/>
-    <sheet name="CP-VAL-CP-004" sheetId="14" r:id="rId4"/>
+    <sheet name="CP-VAL-CP-003" sheetId="14" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
   <si>
     <t>Nombre Proyecto:</t>
   </si>
@@ -147,12 +146,6 @@
   </si>
   <si>
     <t>CP-VAL-CP-003</t>
-  </si>
-  <si>
-    <t>CP-VAL-CP-005</t>
-  </si>
-  <si>
-    <t>código con terminación que no existe para la provincia</t>
   </si>
   <si>
     <t>Conocemos el nombre de la provincia a la que pertenece el código y la terminación de este existe para la provincia</t>
@@ -321,15 +314,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -349,15 +351,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -379,37 +372,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -831,10 +794,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -846,10 +809,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -859,10 +822,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -870,21 +833,21 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -906,73 +869,73 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="C11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="C12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -984,10 +947,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="21"/>
+      <c r="C16" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="13"/>
       <c r="E16" s="7" t="s">
         <v>23</v>
       </c>
@@ -999,10 +962,10 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="21"/>
+      <c r="C17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="7" t="s">
         <v>23</v>
       </c>
@@ -1014,8 +977,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1032,65 +995,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="C21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1101,13 +1064,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="B4:C4"/>
@@ -1124,15 +1080,22 @@
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="B6:F8"/>
     <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Aprobado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pendiente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1158,10 +1121,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1173,10 +1136,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1186,10 +1149,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1197,17 +1160,17 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -1233,73 +1196,73 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1311,10 +1274,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="7" t="s">
         <v>23</v>
       </c>
@@ -1326,8 +1289,8 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -1335,8 +1298,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1353,65 +1316,389 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="14"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Aprobado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Pendiente"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Error"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33690C3C-49D4-4574-A399-1EE508E45F16}">
+  <dimension ref="B2:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>3</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
+        <v>2</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="17"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1447,653 +1734,6 @@
     <mergeCell ref="B26:C26"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>"Aprobado"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B7E240C-6ABF-49B1-B6D3-DA6A961E2917}">
-  <dimension ref="B2:F26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>2</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>3</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
-        <v>3</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="B26:C26"/>
-  </mergeCells>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"Aprobado"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"Pendiente"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"Error"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33690C3C-49D4-4574-A399-1EE508E45F16}">
-  <dimension ref="B2:J26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>2</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>3</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <v>1</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
-        <v>2</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
-        <v>3</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
-  </mergeCells>
-  <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Aprobado"</formula>
     </cfRule>

</xml_diff>